<commit_message>
implemented saving and modification of dataset
</commit_message>
<xml_diff>
--- a/example_dat_3.xlsx
+++ b/example_dat_3.xlsx
@@ -8,7 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DATA_SET" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="PATIENT" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="PATHOGEN" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -49,19 +51,50 @@
     <t xml:space="preserve">DIAL</t>
   </si>
   <si>
+    <t xml:space="preserve">2019-12-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:23:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
     <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAT0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATHOGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="166" formatCode="H:MM"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -83,6 +116,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,17 +168,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -157,112 +194,205 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6:H6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>43808</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>0.266666666666667</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1000</v>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>60</v>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>43808</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>0.647916666666667</v>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>